<commit_message>
add wireframes and modify some user_stories
</commit_message>
<xml_diff>
--- a/user_stories/01_page_de_connexion/Récupération_mot_de_passe_utilisateur.xlsx
+++ b/user_stories/01_page_de_connexion/Récupération_mot_de_passe_utilisateur.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbochard/Code/Openclassrooms/Projet/P03_Learnathome/user_stories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbochard/Code/Openclassrooms/Projet/P03_Learnathome/user_stories/01_page_de_connexion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E042BBA1-D464-7B41-95B9-5C2F5051D0DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E946B657-F15F-0846-A658-33019246FBC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="2900" windowWidth="27640" windowHeight="16940" xr2:uid="{20CC645F-DF2E-7444-83CB-333C81B895F0}"/>
+    <workbookView xWindow="4900" yWindow="2680" windowWidth="27640" windowHeight="16940" xr2:uid="{20CC645F-DF2E-7444-83CB-333C81B895F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>En tant que</t>
   </si>
@@ -57,19 +57,28 @@
     <t>récupérer mon mot de passe</t>
   </si>
   <si>
-    <t>accéder de pouvoir me connecter à mon compte</t>
-  </si>
-  <si>
-    <t>L'utilisateur récupère son mon de passe en renseignant son identifiant</t>
-  </si>
-  <si>
-    <t>rentre mon identifiant et que je valide</t>
-  </si>
-  <si>
-    <t>je récupère mon mot de passe</t>
-  </si>
-  <si>
     <t>je suis un utilisateur déconnecté et que je suis sur la page de connexion</t>
+  </si>
+  <si>
+    <t>me connecter à mon compte</t>
+  </si>
+  <si>
+    <t>L'utilisateur récupère son mon de passe</t>
+  </si>
+  <si>
+    <t>clique sur le lien "Récupération de mot de passe"</t>
+  </si>
+  <si>
+    <t>je suis redirigé vers la page de récupération de mot de passe</t>
+  </si>
+  <si>
+    <t>je suis sur la page de récupération de mot de passe</t>
+  </si>
+  <si>
+    <t>renseigne mon identifiant</t>
+  </si>
+  <si>
+    <t>je reçoit un email avec mon mot de passe</t>
   </si>
 </sst>
 </file>
@@ -112,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -233,6 +242,54 @@
       </right>
       <top/>
       <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -241,14 +298,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,6 +328,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -593,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B85EFE0-DF4C-9D41-859B-7ADB876B1EB7}">
-  <dimension ref="B1:C11"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,73 +675,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:3" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:3" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+    <row r="4" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="2:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="2:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="C13" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>

</xml_diff>